<commit_message>
Obtain list of movies
Co-Authored-By: bzou153 <62585949+bzou153@users.noreply.github.com>
Co-Authored-By: Terry3080 <100814032+Terry3080@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/movie-information.xlsx
+++ b/movie-information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maggi\Documents\GitHub\rpa-solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13640B3A-9B42-441A-8D4B-38FF28B9551C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26392E7D-2ECC-461A-B362-473C298B8A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="11400" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Director</t>
   </si>
   <si>
-    <t>James Cameron</t>
-  </si>
-  <si>
-    <t>Steven Speilberg</t>
-  </si>
-  <si>
-    <t>Lana Wachowski</t>
-  </si>
-  <si>
-    <t>Lilly Wachowski</t>
+    <t>Steven Spielberg</t>
   </si>
 </sst>
 </file>
@@ -357,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,26 +366,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add try/catch and clean up
</commit_message>
<xml_diff>
--- a/movie-information.xlsx
+++ b/movie-information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maggi\Documents\GitHub\rpa-solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26392E7D-2ECC-461A-B362-473C298B8A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FE1565-6E43-4EB9-82DD-FCF2AC12B4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15720" yWindow="1680" windowWidth="11400" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <t>Director</t>
   </si>
   <si>
-    <t>Steven Spielberg</t>
+    <t>ur mom</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>